<commit_message>
Fixed VPP file, up do date modify
</commit_message>
<xml_diff>
--- a/DataModel/orgchart_datamodel.xlsx
+++ b/DataModel/orgchart_datamodel.xlsx
@@ -4,14 +4,15 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="accounts" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="accounts_companies" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="cities" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="companies" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="countries" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="employees" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="employees_hierarchies" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="history" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="requests" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="roles" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="accounts_companies" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="cities" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="companies" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="countries" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="employees" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="employees_hierarchies" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="history" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="requests" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -66,21 +67,24 @@
     <t>password</t>
   </si>
   <si>
-    <t>account_role</t>
+    <t>role_fk</t>
+  </si>
+  <si>
+    <t>roles.id</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
   </si>
   <si>
     <t>TINYINT</t>
   </si>
   <si>
-    <t>0 = read only per altre aziende, richieste per tua azienda e per tuoi dati 
-1 = approvazione richieste per tua azienda e impiegati tua azienda 
-2 = system admin</t>
-  </si>
-  <si>
-    <t>is_deleted</t>
-  </si>
-  <si>
     <t>0 = not deleted, 1 = deleted</t>
+  </si>
+  <si>
+    <t>ROLE_USER, 
+ROLE_COMPANY_ADMIN, 
+ROLE_SYSADMIN</t>
   </si>
   <si>
     <t>account_fk</t>
@@ -207,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -218,6 +222,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font/>
   </fonts>
@@ -241,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -269,13 +277,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -290,6 +301,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -601,28 +616,30 @@
       <c r="D4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" ht="67.5" customHeight="1">
+    <row r="5">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="H5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="8">
         <v>1.0</v>
@@ -635,13 +652,263 @@
       <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G5"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.0"/>
+    <col customWidth="1" min="8" max="8" width="31.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1000.0</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="G6" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8">
+        <v>255.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G6"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="8" width="26.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8">
+        <v>50.0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6">
+      <c r="C6" s="8"/>
+      <c r="D6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -697,40 +964,40 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="G3" s="10" t="s">
-        <v>21</v>
+      <c r="G3" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="G4" s="10" t="s">
-        <v>23</v>
+      <c r="G4" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8">
         <v>1.0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -738,7 +1005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -807,14 +1074,14 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="G4" s="11" t="s">
-        <v>27</v>
+      <c r="G4" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -899,7 +1166,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
@@ -912,7 +1179,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -920,13 +1187,13 @@
       <c r="C5" s="8"/>
       <c r="D5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="10" t="s">
-        <v>30</v>
+      <c r="G5" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -939,12 +1206,12 @@
       </c>
       <c r="F6" s="6"/>
       <c r="H6" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -958,15 +1225,15 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C8" s="8">
         <v>1.0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="13">
         <v>0.0</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -3954,7 +4221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4024,7 +4291,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
@@ -4039,7 +4306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4096,7 +4363,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
@@ -4109,7 +4376,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
@@ -4122,10 +4389,10 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="7" t="s">
@@ -4135,10 +4402,10 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="8">
         <v>1.0</v>
@@ -4150,7 +4417,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -4160,13 +4427,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="10" t="s">
-        <v>30</v>
+      <c r="G7" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -4176,16 +4443,16 @@
         <v>10</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="10" t="s">
-        <v>23</v>
+      <c r="G8" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="8">
         <v>1.0</v>
@@ -4202,7 +4469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4260,7 +4527,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -4268,13 +4535,13 @@
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="10" t="s">
-        <v>42</v>
+      <c r="G3" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -4282,23 +4549,23 @@
       <c r="C4" s="4"/>
       <c r="D4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="10" t="s">
-        <v>42</v>
+      <c r="G4" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="4">
         <v>0.0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4306,7 +4573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4362,7 +4629,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -4371,7 +4638,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
@@ -4382,42 +4649,42 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="8">
         <v>1.0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="G6" s="10" t="s">
-        <v>21</v>
+      <c r="G6" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
@@ -4429,159 +4696,4 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="15.0"/>
-    <col customWidth="1" min="8" max="8" width="31.38"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="F2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1000.0</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="G6" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="H8" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="8">
-        <v>255.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="G6"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>